<commit_message>
Applied patch 10392 (issue with Auto Filters)
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AutoFilter.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/AutoFilter.xlsx
@@ -8,7 +8,10 @@
   <x:sheets>
     <x:sheet name="AutoFilter" sheetId="2" r:id="rId2"/>
   </x:sheets>
-  <x:definedNames/>
+  <x:definedNames>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AutoFilter'!$A$1:$A$4</x:definedName>
+    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0">'AutoFilter'!$A$1:$A$4</x:definedName>
+  </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>

</xml_diff>